<commit_message>
Added menu and inventory
</commit_message>
<xml_diff>
--- a/Actual Amazon.xlsx
+++ b/Actual Amazon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="742" documentId="8_{1ECD4A31-459F-47A0-92D1-5EEA5A332C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F7EF67-7FE0-4CE9-9FAD-938B766378BD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B7C5EC9D-A0EA-4DE3-A89D-E349095D9B5D}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{B7C5EC9D-A0EA-4DE3-A89D-E349095D9B5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,6 +567,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -868,19 +872,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED2C0C1-C4AF-4428-91C7-E2D64E7B4045}">
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.109375" style="16"/>
-    <col min="4" max="4" width="9.109375" style="15"/>
-    <col min="6" max="6" width="9.109375" style="4"/>
-    <col min="10" max="10" width="9.109375" style="6"/>
+    <col min="3" max="3" width="9.140625" style="16"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="10" max="10" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>592.04000000000008</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1113,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>727.61</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1379,7 +1383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1523,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>101.64999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E19">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1869,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1919,7 +1923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1966,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2097,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2181,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2223,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2312,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2362,7 +2366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2416,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2504,7 +2508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2569,7 +2573,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>52</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>2044.66</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>235.82999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>159.32999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2930,7 +2934,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -3002,7 +3006,7 @@
         <v>392.84999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T41">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3032,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>431.27</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -3236,7 +3240,7 @@
         <v>78.61</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -3302,7 +3306,7 @@
         <v>165.66</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -3368,7 +3372,7 @@
         <v>849.92</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -3431,7 +3435,7 @@
         <v>159.30000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>73.92</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -3567,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -3627,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -3690,7 +3694,7 @@
         <v>53.11</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -3750,7 +3754,7 @@
         <v>49.67</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E53">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -3799,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="T54">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3829,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="U55">
         <f t="shared" si="18"/>
         <v>0</v>
@@ -3855,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="U56">
         <f>T56-F52</f>
         <v>-16.989999999999998</v>
@@ -3881,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -3930,7 +3934,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3979,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H59" s="9"/>
       <c r="I59">
         <f>SUM(H59*C73)</f>
@@ -4011,7 +4015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -4056,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -4101,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E62">
         <f t="shared" ref="E62:E72" si="21">C62+D62</f>
         <v>0</v>
@@ -4111,7 +4115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -4130,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -4152,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -4175,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>92</v>
       </c>
@@ -4197,7 +4201,7 @@
         <v>39.480000000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>93</v>
       </c>
@@ -4222,7 +4226,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>94</v>
       </c>
@@ -4245,7 +4249,7 @@
         <v>18.960000000000036</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>53</v>
       </c>
@@ -4258,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -4280,7 +4284,7 @@
         <v>161.1</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>95</v>
       </c>
@@ -4299,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>96</v>
       </c>
@@ -4321,7 +4325,7 @@
         <v>79.959999999999994</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>58</v>
       </c>
@@ -4340,7 +4344,7 @@
         <v>59.84</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>98</v>
       </c>
@@ -4365,9 +4369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3689384-5F96-44CE-B88B-E44A17763C52}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>